<commit_message>
Alright, got a few things fixed in the underlying model that were causing an issue with depreciation
</commit_message>
<xml_diff>
--- a/Farm_Outputs.xlsx
+++ b/Farm_Outputs.xlsx
@@ -2830,13 +2830,13 @@
         <v>157046.8</v>
       </c>
       <c r="E2" t="n">
-        <v>81579.9545508088</v>
+        <v>92585.2570508088</v>
       </c>
       <c r="F2" t="n">
-        <v>238626.754550809</v>
+        <v>249632.057050809</v>
       </c>
       <c r="G2" t="n">
-        <v>238626.754550809</v>
+        <v>249632.057050809</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -2883,13 +2883,13 @@
         <v>16140.4</v>
       </c>
       <c r="E3" t="n">
-        <v>82018.9545508088</v>
+        <v>93084.9820508088</v>
       </c>
       <c r="F3" t="n">
-        <v>98159.3545508088</v>
+        <v>109225.382050809</v>
       </c>
       <c r="G3" t="n">
-        <v>336786.109101618</v>
+        <v>358857.439101618</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -2936,13 +2936,13 @@
         <v>105846.28125</v>
       </c>
       <c r="E4" t="n">
-        <v>145487.349550809</v>
+        <v>103027.008300809</v>
       </c>
       <c r="F4" t="n">
-        <v>251333.630800809</v>
+        <v>208873.289550809</v>
       </c>
       <c r="G4" t="n">
-        <v>588119.739902426</v>
+        <v>567730.728652426</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -2986,46 +2986,46 @@
         <v>28</v>
       </c>
       <c r="D5" t="n">
-        <v>36194.28125</v>
+        <v>35157.78125</v>
       </c>
       <c r="E5" t="n">
-        <v>208949.744550809</v>
+        <v>104069.034550809</v>
       </c>
       <c r="F5" t="n">
-        <v>245144.025800809</v>
+        <v>139226.815800809</v>
       </c>
       <c r="G5" t="n">
-        <v>833263.765703235</v>
+        <v>706957.544453235</v>
       </c>
       <c r="H5" t="n">
-        <v>66992.1875</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>100.620367314639</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>3.96143392321407</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>23.2279079255236</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0512087103707678</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>19.5279278224285</v>
-      </c>
-      <c r="N5" t="n">
-        <v>3.65929274664764</v>
-      </c>
-      <c r="O5" t="n">
-        <v>12.4382229749288</v>
-      </c>
-      <c r="P5" t="n">
-        <v>71.4584046376713</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>242.892720493681</v>
+        <v>0</v>
+      </c>
+      <c r="N5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="O5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P5" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q5" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="6">
@@ -3039,46 +3039,46 @@
         <v>29</v>
       </c>
       <c r="D6" t="n">
-        <v>43047.5</v>
+        <v>41675</v>
       </c>
       <c r="E6" t="n">
         <v>104069.034550809</v>
       </c>
       <c r="F6" t="n">
-        <v>147116.534550809</v>
+        <v>145744.034550809</v>
       </c>
       <c r="G6" t="n">
-        <v>980380.300254044</v>
+        <v>852701.579004044</v>
       </c>
       <c r="H6" t="n">
-        <v>66992.1875</v>
+        <v>58618.1640625</v>
       </c>
       <c r="I6" t="n">
-        <v>100.620367314639</v>
+        <v>120.321920402265</v>
       </c>
       <c r="J6" t="n">
-        <v>3.96143392321407</v>
+        <v>4.73708603842923</v>
       </c>
       <c r="K6" t="n">
-        <v>23.2279079255236</v>
+        <v>42.5074125817755</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0512087103707678</v>
+        <v>0.0937126919260338</v>
       </c>
       <c r="M6" t="n">
-        <v>19.5279278224285</v>
+        <v>10.6709131863301</v>
       </c>
       <c r="N6" t="n">
-        <v>2.19602523877592</v>
+        <v>2.48632888596465</v>
       </c>
       <c r="O6" t="n">
-        <v>7.31712410685234</v>
+        <v>14.5467124848004</v>
       </c>
       <c r="P6" t="n">
-        <v>42.8838223590475</v>
+        <v>26.5313996947935</v>
       </c>
       <c r="Q6" t="n">
-        <v>142.888271426364</v>
+        <v>155.226706071808</v>
       </c>
     </row>
     <row r="7">
@@ -3092,46 +3092,46 @@
         <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>43047.5</v>
+        <v>41675</v>
       </c>
       <c r="E7" t="n">
         <v>104069.034550809</v>
       </c>
       <c r="F7" t="n">
-        <v>147116.534550809</v>
+        <v>145744.034550809</v>
       </c>
       <c r="G7" t="n">
-        <v>1127496.83480485</v>
+        <v>998445.613554853</v>
       </c>
       <c r="H7" t="n">
-        <v>66992.1875</v>
+        <v>58618.1640625</v>
       </c>
       <c r="I7" t="n">
-        <v>100.620367314639</v>
+        <v>120.321920402265</v>
       </c>
       <c r="J7" t="n">
-        <v>3.96143392321407</v>
+        <v>4.73708603842923</v>
       </c>
       <c r="K7" t="n">
-        <v>23.2279079255236</v>
+        <v>42.5074125817755</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0512087103707678</v>
+        <v>0.0937126919260338</v>
       </c>
       <c r="M7" t="n">
-        <v>19.5279278224285</v>
+        <v>10.6709131863301</v>
       </c>
       <c r="N7" t="n">
-        <v>2.19602523877592</v>
+        <v>2.48632888596465</v>
       </c>
       <c r="O7" t="n">
-        <v>5.61009115082687</v>
+        <v>8.5165206853825</v>
       </c>
       <c r="P7" t="n">
-        <v>42.8838223590475</v>
+        <v>26.5313996947935</v>
       </c>
       <c r="Q7" t="n">
-        <v>109.553455070592</v>
+        <v>90.8790528833008</v>
       </c>
     </row>
     <row r="8">
@@ -3145,46 +3145,46 @@
         <v>31</v>
       </c>
       <c r="D8" t="n">
-        <v>43047.5</v>
+        <v>41675</v>
       </c>
       <c r="E8" t="n">
         <v>104069.034550809</v>
       </c>
       <c r="F8" t="n">
-        <v>147116.534550809</v>
+        <v>145744.034550809</v>
       </c>
       <c r="G8" t="n">
-        <v>1274613.36935566</v>
+        <v>1144189.64810566</v>
       </c>
       <c r="H8" t="n">
-        <v>66992.1875</v>
+        <v>58618.1640625</v>
       </c>
       <c r="I8" t="n">
-        <v>100.620367314639</v>
+        <v>120.321920402265</v>
       </c>
       <c r="J8" t="n">
-        <v>3.96143392321407</v>
+        <v>4.73708603842923</v>
       </c>
       <c r="K8" t="n">
-        <v>23.2279079255236</v>
+        <v>42.5074125817755</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0512087103707678</v>
+        <v>0.0937126919260338</v>
       </c>
       <c r="M8" t="n">
-        <v>19.5279278224285</v>
+        <v>10.6709131863301</v>
       </c>
       <c r="N8" t="n">
-        <v>2.19602523877592</v>
+        <v>2.48632888596465</v>
       </c>
       <c r="O8" t="n">
-        <v>4.75657467281413</v>
+        <v>6.50645675224322</v>
       </c>
       <c r="P8" t="n">
-        <v>42.8838223590475</v>
+        <v>26.5313996947935</v>
       </c>
       <c r="Q8" t="n">
-        <v>92.8860468927058</v>
+        <v>69.4298351537983</v>
       </c>
     </row>
     <row r="9">
@@ -3198,46 +3198,46 @@
         <v>32</v>
       </c>
       <c r="D9" t="n">
-        <v>43047.5</v>
+        <v>41675</v>
       </c>
       <c r="E9" t="n">
         <v>104069.034550809</v>
       </c>
       <c r="F9" t="n">
-        <v>147116.534550809</v>
+        <v>145744.034550809</v>
       </c>
       <c r="G9" t="n">
-        <v>1421729.90390647</v>
+        <v>1289933.68265647</v>
       </c>
       <c r="H9" t="n">
-        <v>66992.1875</v>
+        <v>58618.1640625</v>
       </c>
       <c r="I9" t="n">
-        <v>100.620367314639</v>
+        <v>120.321920402265</v>
       </c>
       <c r="J9" t="n">
-        <v>3.96143392321407</v>
+        <v>4.73708603842923</v>
       </c>
       <c r="K9" t="n">
-        <v>23.2279079255236</v>
+        <v>42.5074125817755</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0512087103707678</v>
+        <v>0.0937126919260338</v>
       </c>
       <c r="M9" t="n">
-        <v>19.5279278224285</v>
+        <v>10.6709131863301</v>
       </c>
       <c r="N9" t="n">
-        <v>2.19602523877592</v>
+        <v>2.48632888596465</v>
       </c>
       <c r="O9" t="n">
-        <v>4.24446478600649</v>
+        <v>5.50142478567358</v>
       </c>
       <c r="P9" t="n">
-        <v>42.8838223590475</v>
+        <v>26.5313996947935</v>
       </c>
       <c r="Q9" t="n">
-        <v>82.8856019859741</v>
+        <v>58.7052262890471</v>
       </c>
     </row>
     <row r="10">
@@ -3251,46 +3251,46 @@
         <v>33</v>
       </c>
       <c r="D10" t="n">
-        <v>43047.5</v>
+        <v>41675</v>
       </c>
       <c r="E10" t="n">
         <v>104069.034550809</v>
       </c>
       <c r="F10" t="n">
-        <v>147116.534550809</v>
+        <v>145744.034550809</v>
       </c>
       <c r="G10" t="n">
-        <v>1568846.43845728</v>
+        <v>1435677.71720728</v>
       </c>
       <c r="H10" t="n">
-        <v>66992.1875</v>
+        <v>58618.1640625</v>
       </c>
       <c r="I10" t="n">
-        <v>100.620367314639</v>
+        <v>120.321920402265</v>
       </c>
       <c r="J10" t="n">
-        <v>3.96143392321407</v>
+        <v>4.73708603842923</v>
       </c>
       <c r="K10" t="n">
-        <v>23.2279079255236</v>
+        <v>42.5074125817755</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0512087103707678</v>
+        <v>0.0937126919260338</v>
       </c>
       <c r="M10" t="n">
-        <v>19.5279278224285</v>
+        <v>10.6709131863301</v>
       </c>
       <c r="N10" t="n">
-        <v>2.19602523877592</v>
+        <v>2.48632888596465</v>
       </c>
       <c r="O10" t="n">
-        <v>3.90305819480139</v>
+        <v>4.89840560573179</v>
       </c>
       <c r="P10" t="n">
-        <v>42.8838223590475</v>
+        <v>26.5313996947935</v>
       </c>
       <c r="Q10" t="n">
-        <v>76.2186387148197</v>
+        <v>52.2704609701964</v>
       </c>
     </row>
     <row r="11">
@@ -3304,46 +3304,46 @@
         <v>34</v>
       </c>
       <c r="D11" t="n">
-        <v>43047.5</v>
+        <v>41675</v>
       </c>
       <c r="E11" t="n">
         <v>104069.034550809</v>
       </c>
       <c r="F11" t="n">
-        <v>147116.534550809</v>
+        <v>145744.034550809</v>
       </c>
       <c r="G11" t="n">
-        <v>1715962.97300809</v>
+        <v>1581421.75175809</v>
       </c>
       <c r="H11" t="n">
-        <v>66992.1875</v>
+        <v>58618.1640625</v>
       </c>
       <c r="I11" t="n">
-        <v>100.620367314639</v>
+        <v>120.321920402265</v>
       </c>
       <c r="J11" t="n">
-        <v>3.96143392321407</v>
+        <v>4.73708603842923</v>
       </c>
       <c r="K11" t="n">
-        <v>23.2279079255236</v>
+        <v>42.5074125817755</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0512087103707678</v>
+        <v>0.0937126919260338</v>
       </c>
       <c r="M11" t="n">
-        <v>19.5279278224285</v>
+        <v>10.6709131863301</v>
       </c>
       <c r="N11" t="n">
-        <v>2.19602523877592</v>
+        <v>2.48632888596465</v>
       </c>
       <c r="O11" t="n">
-        <v>3.65919634394061</v>
+        <v>4.49639281910393</v>
       </c>
       <c r="P11" t="n">
-        <v>42.8838223590475</v>
+        <v>26.5313996947935</v>
       </c>
       <c r="Q11" t="n">
-        <v>71.4565220925665</v>
+        <v>47.9806174242959</v>
       </c>
     </row>
     <row r="12">
@@ -3357,46 +3357,46 @@
         <v>35</v>
       </c>
       <c r="D12" t="n">
-        <v>43047.5</v>
+        <v>41675</v>
       </c>
       <c r="E12" t="n">
         <v>104069.034550809</v>
       </c>
       <c r="F12" t="n">
-        <v>147116.534550809</v>
+        <v>145744.034550809</v>
       </c>
       <c r="G12" t="n">
-        <v>1863079.5075589</v>
+        <v>1727165.7863089</v>
       </c>
       <c r="H12" t="n">
-        <v>66992.1875</v>
+        <v>58618.1640625</v>
       </c>
       <c r="I12" t="n">
-        <v>100.620367314639</v>
+        <v>120.321920402265</v>
       </c>
       <c r="J12" t="n">
-        <v>3.96143392321407</v>
+        <v>4.73708603842923</v>
       </c>
       <c r="K12" t="n">
-        <v>23.2279079255236</v>
+        <v>42.5074125817755</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0512087103707678</v>
+        <v>0.0937126919260338</v>
       </c>
       <c r="M12" t="n">
-        <v>19.5279278224285</v>
+        <v>10.6709131863301</v>
       </c>
       <c r="N12" t="n">
-        <v>2.19602523877592</v>
+        <v>2.48632888596465</v>
       </c>
       <c r="O12" t="n">
-        <v>3.47629995579503</v>
+        <v>4.20924082865547</v>
       </c>
       <c r="P12" t="n">
-        <v>42.8838223590475</v>
+        <v>26.5313996947935</v>
       </c>
       <c r="Q12" t="n">
-        <v>67.8849346258767</v>
+        <v>44.9164434629384</v>
       </c>
     </row>
   </sheetData>
@@ -5468,7 +5468,7 @@
         <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
         <v>133</v>
@@ -5495,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="L16" t="s">
         <v>266</v>
@@ -5512,43 +5512,43 @@
         <v>157</v>
       </c>
       <c r="B17" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C17" t="s">
         <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>134</v>
       </c>
       <c r="E17" t="s">
         <v>240</v>
       </c>
       <c r="F17" t="n">
-        <v>428.75</v>
+        <v>15.9127272727273</v>
       </c>
       <c r="G17" t="n">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="I17" t="n">
-        <v>1250</v>
+        <v>275</v>
       </c>
       <c r="J17" t="n">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="L17" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="M17" t="n">
-        <v>432</v>
+        <v>16</v>
       </c>
       <c r="N17" t="n">
-        <v>6480</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18">
@@ -5556,43 +5556,43 @@
         <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>200</v>
+        <v>134</v>
       </c>
       <c r="E18" t="s">
         <v>240</v>
       </c>
       <c r="F18" t="n">
-        <v>120</v>
+        <v>15.9127272727273</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="I18" t="n">
-        <v>10</v>
+        <v>275</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="L18" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="M18" t="n">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19">
@@ -5600,10 +5600,10 @@
         <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
         <v>200</v>
@@ -5612,31 +5612,31 @@
         <v>240</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>375.15625</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="s">
         <v>242</v>
       </c>
       <c r="L19" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="20">
@@ -5644,7 +5644,7 @@
         <v>162</v>
       </c>
       <c r="B20" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C20" t="s">
         <v>199</v>
@@ -5656,7 +5656,7 @@
         <v>240</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -5665,19 +5665,19 @@
         <v>273</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="L20" t="s">
         <v>274</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="N20" t="n">
         <v>0</v>
@@ -5688,7 +5688,7 @@
         <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C21" t="s">
         <v>199</v>
@@ -5715,7 +5715,7 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="L21" t="s">
         <v>274</v>
@@ -5724,6 +5724,94 @@
         <v>0</v>
       </c>
       <c r="N21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" t="s">
+        <v>276</v>
+      </c>
+      <c r="C22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>273</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>245</v>
+      </c>
+      <c r="L22" t="s">
+        <v>274</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" t="s">
+        <v>277</v>
+      </c>
+      <c r="C23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" t="s">
+        <v>240</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>273</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>278</v>
+      </c>
+      <c r="L23" t="s">
+        <v>274</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5970,7 +6058,7 @@
         <v>284</v>
       </c>
       <c r="I8" t="n">
-        <v>7056</v>
+        <v>6678</v>
       </c>
     </row>
     <row r="9">
@@ -5999,7 +6087,7 @@
         <v>284</v>
       </c>
       <c r="I9" t="n">
-        <v>3360</v>
+        <v>3180</v>
       </c>
     </row>
   </sheetData>
@@ -6238,7 +6326,7 @@
         <v>134</v>
       </c>
       <c r="E9" t="n">
-        <v>8400</v>
+        <v>7950</v>
       </c>
       <c r="F9" t="s">
         <v>232</v>
@@ -6264,7 +6352,7 @@
         <v>134</v>
       </c>
       <c r="E10" t="n">
-        <v>84</v>
+        <v>79.5</v>
       </c>
       <c r="F10" t="s">
         <v>289</v>

</xml_diff>